<commit_message>
test(e2e): Max allowed number of characters in widget input field
</commit_message>
<xml_diff>
--- a/e2e/RasaChatbotWidgetTestCases.xlsx
+++ b/e2e/RasaChatbotWidgetTestCases.xlsx
@@ -28,7 +28,8 @@
     <sheet name="TC018" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="TC019" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="TC020" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="Test Case 2 (2)" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="TC021" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="Test Case 2 (2)" sheetId="23" state="visible" r:id="rId23"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
   <si>
     <t>Automated</t>
   </si>
@@ -1379,6 +1380,88 @@
   </si>
   <si>
     <t xml:space="preserve">On each message either from user input or from chatbot response there is a timestamp displayed. </t>
+  </si>
+  <si>
+    <t>TC021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share messages between tabs</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Widget is built and chatbot is up and trained and connected with widget. Before getting widget up set the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>server-url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> property to target chatbot server with defined and trainned flow. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>server-url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> property is mandatory in order to get widget loaded. Also </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>server-id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> prop needs to be set with a string as a value.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">User opens a widget and starts a conversation. When new tab/tabs are opened chat history and new messages are visible on other tabs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User opens 2 tabs with widget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabs are opened</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User sends message in one tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chat history is synced between the opened tabs</t>
   </si>
 </sst>
 </file>
@@ -2504,7 +2587,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>31748</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1416048" cy="2216147"/>
     <xdr:pic>
@@ -2533,9 +2616,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>609598</xdr:colOff>
+      <xdr:colOff>609597</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2197098" cy="1025523"/>
     <xdr:pic>
@@ -2564,11 +2647,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>609598</xdr:colOff>
+      <xdr:colOff>609597</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2443165" cy="1955799"/>
+    <xdr:ext cx="2443164" cy="1955799"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1538479734" name=""/>
@@ -2602,7 +2685,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1416048" cy="2216147"/>
     <xdr:pic>
@@ -2633,7 +2716,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>577848</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2280091" cy="1015998"/>
     <xdr:pic>
@@ -2649,7 +2732,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
-          <a:off x="1794117" y="4528038"/>
+          <a:off x="1794116" y="4528038"/>
           <a:ext cx="2280091" cy="1015998"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2662,11 +2745,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>609598</xdr:colOff>
+      <xdr:colOff>609597</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2133598" cy="1974713"/>
+    <xdr:ext cx="2133598" cy="1974711"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="899296141" name=""/>
@@ -2681,7 +2764,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
           <a:off x="4256942" y="4528038"/>
-          <a:ext cx="2133598" cy="1974713"/>
+          <a:ext cx="2133598" cy="1974712"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2700,7 +2783,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1416048" cy="2216147"/>
     <xdr:pic>
@@ -2729,9 +2812,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>609598</xdr:colOff>
+      <xdr:colOff>609597</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2006672" cy="901698"/>
     <xdr:pic>
@@ -2760,11 +2843,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>609598</xdr:colOff>
+      <xdr:colOff>609597</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1907573" cy="1485898"/>
+    <xdr:ext cx="1907572" cy="1485898"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="163283211" name=""/>
@@ -2791,9 +2874,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>609598</xdr:colOff>
+      <xdr:colOff>609597</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2051304" cy="2419348"/>
     <xdr:pic>
@@ -2829,7 +2912,7 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1416048" cy="2216147"/>
     <xdr:pic>
@@ -2858,9 +2941,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>609598</xdr:colOff>
+      <xdr:colOff>609597</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2416478" cy="1108073"/>
     <xdr:pic>
@@ -2889,11 +2972,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>609598</xdr:colOff>
+      <xdr:colOff>609597</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2387598" cy="2387598"/>
+    <xdr:ext cx="2387597" cy="2387597"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="387836096" name=""/>
@@ -2920,11 +3003,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>609598</xdr:colOff>
+      <xdr:colOff>609597</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>165098</xdr:rowOff>
+      <xdr:rowOff>165097</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2387763" cy="2393947"/>
+    <xdr:ext cx="2387762" cy="2393947"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1019781314" name=""/>
@@ -3089,7 +3172,7 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>163284</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2296146" cy="1034141"/>
+    <xdr:ext cx="2296145" cy="1034141"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="95849097" name=""/>
@@ -3116,7 +3199,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>612320</xdr:colOff>
+      <xdr:colOff>612319</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>163284</xdr:rowOff>
     </xdr:from>
@@ -3147,7 +3230,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>612320</xdr:colOff>
+      <xdr:colOff>612319</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>163284</xdr:rowOff>
     </xdr:from>
@@ -3249,7 +3332,7 @@
       <xdr:row>27</xdr:row>
       <xdr:rowOff>163284</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2428873" cy="1883351"/>
+    <xdr:ext cx="2428873" cy="1883349"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1961853996" name=""/>
@@ -3264,7 +3347,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="0" flipV="0">
           <a:off x="4256942" y="4528038"/>
-          <a:ext cx="2428873" cy="1883351"/>
+          <a:ext cx="2428872" cy="1883351"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5020,7 +5103,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="F18" activeCellId="0" sqref="F18:K20"/>
     </sheetView>
   </sheetViews>
@@ -5056,7 +5139,7 @@
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="11" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
@@ -9313,6 +9396,402 @@
         <v>3</v>
       </c>
       <c r="B1" s="4"/>
+      <c r="C1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" ht="12.75">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" ht="12.75">
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" ht="12.75">
+      <c r="A4" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" ht="12.75">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" ht="12.75">
+      <c r="A6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="22"/>
+    </row>
+    <row r="7" ht="12.75">
+      <c r="A7" s="23">
+        <v>1</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="23">
+        <v>1</v>
+      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" ht="12.75">
+      <c r="A8" s="27">
+        <v>2</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="27">
+        <v>2</v>
+      </c>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+    </row>
+    <row r="9" ht="12.75">
+      <c r="A9" s="27">
+        <v>3</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="27">
+        <v>3</v>
+      </c>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
+    </row>
+    <row r="10" ht="12.75">
+      <c r="A10" s="27">
+        <v>4</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="27">
+        <v>4</v>
+      </c>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
+    </row>
+    <row r="11" ht="12.75">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" ht="12.75">
+      <c r="A12" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
+    </row>
+    <row r="14" ht="12.75">
+      <c r="A14" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+    </row>
+    <row r="15" ht="12.75">
+      <c r="A15" s="40"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="44"/>
+    </row>
+    <row r="16" ht="24.75" customHeight="1">
+      <c r="A16" s="23">
+        <v>1</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="26"/>
+    </row>
+    <row r="17" ht="12.75">
+      <c r="A17" s="27">
+        <v>2</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
+    </row>
+    <row r="18" ht="12.75">
+      <c r="A18" s="27">
+        <v>3</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="30"/>
+    </row>
+    <row r="19" ht="12.75">
+      <c r="A19" s="27">
+        <v>4</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="30"/>
+    </row>
+    <row r="20" ht="12.75" customHeight="1">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" ht="12.75" customHeight="1">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="D14:K15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:K19"/>
+  </mergeCells>
+  <dataValidations count="1" disablePrompts="0">
+    <dataValidation sqref="C2" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Sheet1!$A$1:$A$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="1" scale="90" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="65533" verticalDpi="65533" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="F18" activeCellId="0" sqref="F18:K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" customHeight="1"/>
+  <cols>
+    <col customWidth="1" min="1" max="257" style="2" width="9.1406200000000002"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="12.75">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4"/>
       <c r="C1" s="5"/>
       <c r="D1" s="6" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
test(e2e):SocketIO connection is reconnected after more then 5s widget is closed
</commit_message>
<xml_diff>
--- a/e2e/RasaChatbotWidgetTestCases.xlsx
+++ b/e2e/RasaChatbotWidgetTestCases.xlsx
@@ -4,7 +4,7 @@
   <workbookPr hidePivotFieldList="0"/>
   <workbookProtection lockStructure="0" lockWindows="0" workbookPassword="0000"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="12"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -29,7 +29,8 @@
     <sheet name="TC019" sheetId="20" state="visible" r:id="rId20"/>
     <sheet name="TC020" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="TC021" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="Test Case 2 (2)" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="TC022" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="Test Case 2 (2)" sheetId="24" state="visible" r:id="rId24"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
   <si>
     <t>Automated</t>
   </si>
@@ -1462,6 +1463,77 @@
   </si>
   <si>
     <t xml:space="preserve">Chat history is synced between the opened tabs</t>
+  </si>
+  <si>
+    <t>TC022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widget reconnects SocketIO session after 5s</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Widget is built and chatbot is up and trained and connected with widget. Before getting widget up set the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>server-url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> property to target chatbot server with defined and trainned flow. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>server-url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> property is mandatory in order to get widget loaded..</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">User opens a widget and start a conversation. Closes the widget and after 5s or more opens a widget again. New session divider should be visible in session wndow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User sends message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chat bot replies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User closes widget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widget launcher button is visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User waits for 5s or more before opening a widget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widget is opened with chat history and new session divider visible.</t>
   </si>
 </sst>
 </file>
@@ -1834,7 +1906,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="47">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -2307,6 +2379,111 @@
       </bottom>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2363,7 +2540,7 @@
     <xf fontId="19" fillId="0" borderId="9" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="20" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="65">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -2517,6 +2694,33 @@
     </xf>
     <xf fontId="24" fillId="0" borderId="17" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf fontId="24" fillId="0" borderId="38" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="24" fillId="0" borderId="39" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="24" fillId="0" borderId="40" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="24" fillId="0" borderId="41" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="24" fillId="0" borderId="42" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="24" fillId="0" borderId="43" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="24" fillId="0" borderId="44" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="24" fillId="0" borderId="45" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="24" fillId="0" borderId="46" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -9792,6 +9996,412 @@
         <v>3</v>
       </c>
       <c r="B1" s="4"/>
+      <c r="C1" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" ht="12.75">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" ht="12.75">
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" ht="12.75">
+      <c r="A4" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="58"/>
+    </row>
+    <row r="5" ht="12.75">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" ht="12.75">
+      <c r="A6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="22"/>
+    </row>
+    <row r="7" ht="12.75">
+      <c r="A7" s="23">
+        <v>1</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="23">
+        <v>1</v>
+      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" ht="12.75">
+      <c r="A8" s="27">
+        <v>2</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="63"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="27">
+        <v>2</v>
+      </c>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+    </row>
+    <row r="9" ht="12.75">
+      <c r="A9" s="27">
+        <v>3</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="27">
+        <v>3</v>
+      </c>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
+    </row>
+    <row r="10" ht="12.75">
+      <c r="A10" s="27">
+        <v>4</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="27">
+        <v>4</v>
+      </c>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
+    </row>
+    <row r="11" ht="12.75">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" ht="12.75">
+      <c r="A12" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
+    </row>
+    <row r="14" ht="12.75">
+      <c r="A14" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+    </row>
+    <row r="15" ht="12.75">
+      <c r="A15" s="40"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="44"/>
+    </row>
+    <row r="16" ht="24.75" customHeight="1">
+      <c r="A16" s="23">
+        <v>1</v>
+      </c>
+      <c r="B16" s="59" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="61"/>
+      <c r="D16" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="61"/>
+    </row>
+    <row r="17" ht="12.75">
+      <c r="A17" s="27">
+        <v>2</v>
+      </c>
+      <c r="B17" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="64"/>
+      <c r="D17" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="63"/>
+      <c r="K17" s="64"/>
+    </row>
+    <row r="18" ht="12.75">
+      <c r="A18" s="27">
+        <v>3</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="C18" s="48"/>
+      <c r="D18" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="30"/>
+    </row>
+    <row r="19" ht="12.75">
+      <c r="A19" s="27">
+        <v>4</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="48"/>
+      <c r="D19" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="30"/>
+    </row>
+    <row r="20" ht="12.75">
+      <c r="A20" s="27">
+        <v>5</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="C20" s="48"/>
+      <c r="D20" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="30"/>
+    </row>
+    <row r="21" ht="12.75">
+      <c r="A21" s="27"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="31">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="D14:K15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:K21"/>
+  </mergeCells>
+  <dataValidations count="1" disablePrompts="0">
+    <dataValidation sqref="C2" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Sheet1!$A$1:$A$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="1" scale="90" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="65533" verticalDpi="65533" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="F18" activeCellId="0" sqref="F18:K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" customHeight="1"/>
+  <cols>
+    <col customWidth="1" min="1" max="257" style="2" width="9.1406200000000002"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="12.75">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4"/>
       <c r="C1" s="5"/>
       <c r="D1" s="6" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
tests: high resolution images response type use cases
</commit_message>
<xml_diff>
--- a/e2e/RasaChatbotWidgetTestCases.xlsx
+++ b/e2e/RasaChatbotWidgetTestCases.xlsx
@@ -4,7 +4,7 @@
   <workbookPr hidePivotFieldList="0"/>
   <workbookProtection lockStructure="0" lockWindows="0" workbookPassword="0000"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="22"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -30,7 +30,9 @@
     <sheet name="TC020" sheetId="21" state="visible" r:id="rId21"/>
     <sheet name="TC021" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="TC022" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="Test Case 2 (2)" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="TC023" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="TC024" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="Test Case 2 (2)" sheetId="26" state="visible" r:id="rId26"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="175">
   <si>
     <t>Automated</t>
   </si>
@@ -205,7 +207,7 @@
     <t xml:space="preserve">User fills in user input field with "Show me country" and clicks on Send button</t>
   </si>
   <si>
-    <t xml:space="preserve">"Show me country" message is shown in Session window. Chatbot response is text message "No country for old men" followed by image holder and then followed by text message "What else I can help you with?"</t>
+    <t xml:space="preserve">"Show me country" message is shown in Session window. Chatbot response is text message "No country for old men" followed by image holder.</t>
   </si>
   <si>
     <t>TC003</t>
@@ -1534,6 +1536,118 @@
   </si>
   <si>
     <t xml:space="preserve">Widget is opened with chat history and new session divider visible.</t>
+  </si>
+  <si>
+    <t>TC023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response message type: High resolution image</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Widget is built and chatbot is up and trained and connected with widget. Before getting widget up set the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>server-url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> property to target chatbot server with defined and trainned flow. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>server-url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> property is mandatory in order to get widget loaded. Please note that response is defined by chatbot and chatbot flow, purpose of the test is to verify text message response rendering. Server is set to reply with high resolution image.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">User input: "HR_image"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"HR_Image" message is shown in Session window. Chatbot response is text message "You are seeing high resolution image." followed by image holder. Image is rendered correctly.</t>
+  </si>
+  <si>
+    <t>TC024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Response message type: carousel message with high resolution image</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Widget is built and chatbot is up and trained and connected with widget. Before getting widget up set the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>server-url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> property to target chatbot server with defined and trainned flow. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>server-url</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> property is mandatory in order to get widget loaded. Please note that response is defined by chatbot and chatbot flow, purpose of the test is to verify text message response rendering. Set server to respond with high resolution image/images.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">User input: "Carousel_with_high_resolution"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Carousel_with_high_resolution" message is shown in Session window. Chatbot response consists carousel message with scroll arrow on the right side to list carousel message and text message bellow carousel. When listed to the right left arrow is shown as well. </t>
   </si>
 </sst>
 </file>
@@ -1906,7 +2020,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="48">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -2380,9 +2494,7 @@
       <diagonal style="none"/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
+      <left style="none"/>
       <right/>
       <top style="thin">
         <color theme="1"/>
@@ -2408,6 +2520,19 @@
       <right style="thin">
         <color theme="1"/>
       </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
       <top style="thin">
         <color theme="1"/>
       </top>
@@ -2540,7 +2665,7 @@
     <xf fontId="19" fillId="0" borderId="9" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="20" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -2720,6 +2845,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf fontId="24" fillId="0" borderId="46" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="24" fillId="0" borderId="47" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10046,18 +10174,18 @@
       <c r="A4" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="58"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" ht="12.75">
       <c r="A5" s="14"/>
@@ -10097,11 +10225,11 @@
       <c r="A7" s="23">
         <v>1</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="61"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="11"/>
       <c r="F7" s="23">
         <v>1</v>
@@ -10116,11 +10244,11 @@
       <c r="A8" s="27">
         <v>2</v>
       </c>
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="11"/>
       <c r="F8" s="27">
         <v>2</v>
@@ -10231,39 +10359,39 @@
       <c r="A16" s="23">
         <v>1</v>
       </c>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="59" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="60"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="61"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="26"/>
     </row>
     <row r="17" ht="12.75">
       <c r="A17" s="27">
         <v>2</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="64"/>
-      <c r="D17" s="62" t="s">
+      <c r="C17" s="30"/>
+      <c r="D17" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="64"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
     </row>
     <row r="18" ht="12.75">
       <c r="A18" s="27">
@@ -10402,24 +10530,30 @@
         <v>3</v>
       </c>
       <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
+      <c r="C1" s="5" t="s">
+        <v>165</v>
+      </c>
       <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="4"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8"/>
+      <c r="F1" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="58"/>
     </row>
     <row r="2" ht="12.75">
       <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
+      <c r="C2" s="11" t="s">
+        <v>0</v>
+      </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
@@ -10446,16 +10580,18 @@
       <c r="A4" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="8"/>
+      <c r="B4" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="58"/>
     </row>
     <row r="5" ht="12.75">
       <c r="A5" s="14"/>
@@ -10495,28 +10631,32 @@
       <c r="A7" s="23">
         <v>1</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="62"/>
       <c r="E7" s="11"/>
       <c r="F7" s="23">
         <v>1</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
+      <c r="G7" s="60" t="s">
+        <v>168</v>
+      </c>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="62"/>
     </row>
     <row r="8" ht="12.75">
       <c r="A8" s="27">
         <v>2</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
+      <c r="B8" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="64"/>
+      <c r="D8" s="65"/>
       <c r="E8" s="11"/>
       <c r="F8" s="27">
         <v>2</v>
@@ -10578,16 +10718,18 @@
       <c r="A12" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="55"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="33"/>
+      <c r="B12" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="57"/>
+      <c r="K12" s="58"/>
     </row>
     <row r="14" ht="12.75">
       <c r="A14" s="34" t="s">
@@ -10625,61 +10767,77 @@
       <c r="A16" s="23">
         <v>1</v>
       </c>
-      <c r="B16" s="45"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="26"/>
+      <c r="B16" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="62"/>
+      <c r="D16" s="60" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="62"/>
     </row>
     <row r="17" ht="12.75">
       <c r="A17" s="27">
         <v>2</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="48"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="30"/>
+      <c r="B17" s="63" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="65"/>
+      <c r="D17" s="63" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="65"/>
     </row>
     <row r="18" ht="12.75">
       <c r="A18" s="27">
         <v>3</v>
       </c>
-      <c r="B18" s="47"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="30"/>
+      <c r="B18" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="65"/>
+      <c r="D18" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="65"/>
     </row>
     <row r="19" ht="12.75">
       <c r="A19" s="27">
         <v>4</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="30"/>
+      <c r="B19" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="65"/>
+      <c r="D19" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="65"/>
     </row>
     <row r="20" ht="12.75">
       <c r="A20" s="27"/>
@@ -10753,7 +10911,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -10776,14 +10934,14 @@
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="5" t="s">
-        <v>33</v>
+        <v>170</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="7" t="s">
-        <v>34</v>
+        <v>171</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
@@ -10826,7 +10984,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>9</v>
+        <v>172</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -10886,7 +11044,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>35</v>
+        <v>173</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -10906,9 +11064,7 @@
       <c r="F8" s="27">
         <v>2</v>
       </c>
-      <c r="G8" s="28" t="s">
-        <v>36</v>
-      </c>
+      <c r="G8" s="28"/>
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
       <c r="J8" s="29"/>
@@ -10925,9 +11081,7 @@
       <c r="F9" s="27">
         <v>3</v>
       </c>
-      <c r="G9" s="28" t="s">
-        <v>37</v>
-      </c>
+      <c r="G9" s="28"/>
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
       <c r="J9" s="29"/>
@@ -10968,7 +11122,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -11074,11 +11228,11 @@
         <v>4</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="28" t="s">
-        <v>40</v>
+        <v>174</v>
       </c>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
@@ -11115,20 +11269,14 @@
       <c r="K21" s="30"/>
     </row>
     <row r="28" s="50" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A28" s="50" t="s">
-        <v>30</v>
-      </c>
+      <c r="A28" s="50"/>
       <c r="B28" s="50"/>
       <c r="C28" s="50"/>
-      <c r="D28" s="50" t="s">
-        <v>31</v>
-      </c>
+      <c r="D28" s="50"/>
       <c r="E28" s="50"/>
       <c r="F28" s="50"/>
       <c r="G28" s="50"/>
-      <c r="H28" s="50" t="s">
-        <v>32</v>
-      </c>
+      <c r="H28" s="50"/>
       <c r="I28" s="50"/>
       <c r="J28" s="50"/>
       <c r="K28" s="50"/>
@@ -11380,10 +11528,11 @@
       <c r="IW28" s="50"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="H29" s="49"/>
-    </row>
-    <row r="33" ht="12.75" customHeight="1">
-      <c r="E33" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="I29" s="49"/>
+    </row>
+    <row r="45" ht="12.75" customHeight="1">
+      <c r="I45" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -11428,11 +11577,382 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="1" scale="90" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="65533" verticalDpi="65533" copies="1"/>
   <headerFooter/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="F18" activeCellId="0" sqref="F18:K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" customHeight="1"/>
+  <cols>
+    <col customWidth="1" min="1" max="257" style="2" width="9.1406200000000002"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="12.75">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" ht="12.75">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" ht="12.75">
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" ht="12.75">
+      <c r="A4" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" ht="12.75">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" ht="12.75">
+      <c r="A6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="22"/>
+    </row>
+    <row r="7" ht="12.75">
+      <c r="A7" s="23">
+        <v>1</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="23">
+        <v>1</v>
+      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" ht="12.75">
+      <c r="A8" s="27">
+        <v>2</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="27">
+        <v>2</v>
+      </c>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+    </row>
+    <row r="9" ht="12.75">
+      <c r="A9" s="27">
+        <v>3</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="27">
+        <v>3</v>
+      </c>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
+    </row>
+    <row r="10" ht="12.75">
+      <c r="A10" s="27">
+        <v>4</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="27">
+        <v>4</v>
+      </c>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
+    </row>
+    <row r="11" ht="12.75">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" ht="12.75">
+      <c r="A12" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="55"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="33"/>
+    </row>
+    <row r="14" ht="12.75">
+      <c r="A14" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+    </row>
+    <row r="15" ht="12.75">
+      <c r="A15" s="40"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="44"/>
+    </row>
+    <row r="16" ht="24.75" customHeight="1">
+      <c r="A16" s="23">
+        <v>1</v>
+      </c>
+      <c r="B16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="26"/>
+    </row>
+    <row r="17" ht="12.75">
+      <c r="A17" s="27">
+        <v>2</v>
+      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
+    </row>
+    <row r="18" ht="12.75">
+      <c r="A18" s="27">
+        <v>3</v>
+      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="30"/>
+    </row>
+    <row r="19" ht="12.75">
+      <c r="A19" s="27">
+        <v>4</v>
+      </c>
+      <c r="B19" s="47"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="30"/>
+    </row>
+    <row r="20" ht="12.75">
+      <c r="A20" s="27"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="30"/>
+    </row>
+    <row r="21" ht="12.75">
+      <c r="A21" s="27"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="31">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="D14:K15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:K21"/>
+  </mergeCells>
+  <dataValidations count="1" disablePrompts="0">
+    <dataValidation sqref="C2" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Sheet1!$A$1:$A$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="1" scale="90" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="65533" verticalDpi="65533" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -11455,14 +11975,14 @@
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
@@ -11500,7 +12020,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" ht="22.5">
+    <row r="4" ht="12.75">
       <c r="A4" s="53" t="s">
         <v>8</v>
       </c>
@@ -11565,7 +12085,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -11585,7 +12105,9 @@
       <c r="F8" s="27">
         <v>2</v>
       </c>
-      <c r="G8" s="28"/>
+      <c r="G8" s="28" t="s">
+        <v>36</v>
+      </c>
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
       <c r="J8" s="29"/>
@@ -11602,7 +12124,9 @@
       <c r="F9" s="27">
         <v>3</v>
       </c>
-      <c r="G9" s="28"/>
+      <c r="G9" s="28" t="s">
+        <v>37</v>
+      </c>
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
       <c r="J9" s="29"/>
@@ -11643,7 +12167,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -11706,7 +12230,7 @@
       <c r="J16" s="25"/>
       <c r="K16" s="26"/>
     </row>
-    <row r="17" ht="22.5">
+    <row r="17" ht="12.75">
       <c r="A17" s="27">
         <v>2</v>
       </c>
@@ -11725,7 +12249,7 @@
       <c r="J17" s="29"/>
       <c r="K17" s="30"/>
     </row>
-    <row r="18" ht="33.75">
+    <row r="18" ht="12.75">
       <c r="A18" s="27">
         <v>3</v>
       </c>
@@ -11744,16 +12268,16 @@
       <c r="J18" s="29"/>
       <c r="K18" s="30"/>
     </row>
-    <row r="19" ht="33.75">
+    <row r="19" ht="12.75">
       <c r="A19" s="27">
         <v>4</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="28" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
@@ -12055,16 +12579,10 @@
       <c r="IW28" s="50"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="D29" s="49"/>
       <c r="H29" s="49"/>
     </row>
-    <row r="40" ht="12.75" customHeight="1">
-      <c r="H40" s="51" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" ht="12.75" customHeight="1">
-      <c r="H41" s="49"/>
+    <row r="33" ht="12.75" customHeight="1">
+      <c r="E33" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -12113,7 +12631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -12136,14 +12654,14 @@
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="7" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
@@ -12181,7 +12699,7 @@
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
     </row>
-    <row r="4" ht="12.75">
+    <row r="4" ht="22.5">
       <c r="A4" s="53" t="s">
         <v>8</v>
       </c>
@@ -12246,7 +12764,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -12324,7 +12842,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -12387,7 +12905,7 @@
       <c r="J16" s="25"/>
       <c r="K16" s="26"/>
     </row>
-    <row r="17" ht="12.75">
+    <row r="17" ht="22.5">
       <c r="A17" s="27">
         <v>2</v>
       </c>
@@ -12406,7 +12924,7 @@
       <c r="J17" s="29"/>
       <c r="K17" s="30"/>
     </row>
-    <row r="18" ht="12.75">
+    <row r="18" ht="33.75">
       <c r="A18" s="27">
         <v>3</v>
       </c>
@@ -12425,16 +12943,16 @@
       <c r="J18" s="29"/>
       <c r="K18" s="30"/>
     </row>
-    <row r="19" ht="12.75">
+    <row r="19" ht="33.75">
       <c r="A19" s="27">
         <v>4</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="28" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
@@ -12449,688 +12967,6 @@
       <c r="B20" s="47"/>
       <c r="C20" s="48"/>
       <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="30"/>
-    </row>
-    <row r="21" ht="12.75">
-      <c r="A21" s="27"/>
-      <c r="B21" s="47"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="30"/>
-    </row>
-    <row r="28" s="50" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A28" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="J28" s="50"/>
-      <c r="K28" s="50"/>
-      <c r="L28" s="50"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="50"/>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="50"/>
-      <c r="R28" s="50"/>
-      <c r="S28" s="50"/>
-      <c r="T28" s="50"/>
-      <c r="U28" s="50"/>
-      <c r="V28" s="50"/>
-      <c r="W28" s="50"/>
-      <c r="X28" s="50"/>
-      <c r="Y28" s="50"/>
-      <c r="Z28" s="50"/>
-      <c r="AA28" s="50"/>
-      <c r="AB28" s="50"/>
-      <c r="AC28" s="50"/>
-      <c r="AD28" s="50"/>
-      <c r="AE28" s="50"/>
-      <c r="AF28" s="50"/>
-      <c r="AG28" s="50"/>
-      <c r="AH28" s="50"/>
-      <c r="AI28" s="50"/>
-      <c r="AJ28" s="50"/>
-      <c r="AK28" s="50"/>
-      <c r="AL28" s="50"/>
-      <c r="AM28" s="50"/>
-      <c r="AN28" s="50"/>
-      <c r="AO28" s="50"/>
-      <c r="AP28" s="50"/>
-      <c r="AQ28" s="50"/>
-      <c r="AR28" s="50"/>
-      <c r="AS28" s="50"/>
-      <c r="AT28" s="50"/>
-      <c r="AU28" s="50"/>
-      <c r="AV28" s="50"/>
-      <c r="AW28" s="50"/>
-      <c r="AX28" s="50"/>
-      <c r="AY28" s="50"/>
-      <c r="AZ28" s="50"/>
-      <c r="BA28" s="50"/>
-      <c r="BB28" s="50"/>
-      <c r="BC28" s="50"/>
-      <c r="BD28" s="50"/>
-      <c r="BE28" s="50"/>
-      <c r="BF28" s="50"/>
-      <c r="BG28" s="50"/>
-      <c r="BH28" s="50"/>
-      <c r="BI28" s="50"/>
-      <c r="BJ28" s="50"/>
-      <c r="BK28" s="50"/>
-      <c r="BL28" s="50"/>
-      <c r="BM28" s="50"/>
-      <c r="BN28" s="50"/>
-      <c r="BO28" s="50"/>
-      <c r="BP28" s="50"/>
-      <c r="BQ28" s="50"/>
-      <c r="BR28" s="50"/>
-      <c r="BS28" s="50"/>
-      <c r="BT28" s="50"/>
-      <c r="BU28" s="50"/>
-      <c r="BV28" s="50"/>
-      <c r="BW28" s="50"/>
-      <c r="BX28" s="50"/>
-      <c r="BY28" s="50"/>
-      <c r="BZ28" s="50"/>
-      <c r="CA28" s="50"/>
-      <c r="CB28" s="50"/>
-      <c r="CC28" s="50"/>
-      <c r="CD28" s="50"/>
-      <c r="CE28" s="50"/>
-      <c r="CF28" s="50"/>
-      <c r="CG28" s="50"/>
-      <c r="CH28" s="50"/>
-      <c r="CI28" s="50"/>
-      <c r="CJ28" s="50"/>
-      <c r="CK28" s="50"/>
-      <c r="CL28" s="50"/>
-      <c r="CM28" s="50"/>
-      <c r="CN28" s="50"/>
-      <c r="CO28" s="50"/>
-      <c r="CP28" s="50"/>
-      <c r="CQ28" s="50"/>
-      <c r="CR28" s="50"/>
-      <c r="CS28" s="50"/>
-      <c r="CT28" s="50"/>
-      <c r="CU28" s="50"/>
-      <c r="CV28" s="50"/>
-      <c r="CW28" s="50"/>
-      <c r="CX28" s="50"/>
-      <c r="CY28" s="50"/>
-      <c r="CZ28" s="50"/>
-      <c r="DA28" s="50"/>
-      <c r="DB28" s="50"/>
-      <c r="DC28" s="50"/>
-      <c r="DD28" s="50"/>
-      <c r="DE28" s="50"/>
-      <c r="DF28" s="50"/>
-      <c r="DG28" s="50"/>
-      <c r="DH28" s="50"/>
-      <c r="DI28" s="50"/>
-      <c r="DJ28" s="50"/>
-      <c r="DK28" s="50"/>
-      <c r="DL28" s="50"/>
-      <c r="DM28" s="50"/>
-      <c r="DN28" s="50"/>
-      <c r="DO28" s="50"/>
-      <c r="DP28" s="50"/>
-      <c r="DQ28" s="50"/>
-      <c r="DR28" s="50"/>
-      <c r="DS28" s="50"/>
-      <c r="DT28" s="50"/>
-      <c r="DU28" s="50"/>
-      <c r="DV28" s="50"/>
-      <c r="DW28" s="50"/>
-      <c r="DX28" s="50"/>
-      <c r="DY28" s="50"/>
-      <c r="DZ28" s="50"/>
-      <c r="EA28" s="50"/>
-      <c r="EB28" s="50"/>
-      <c r="EC28" s="50"/>
-      <c r="ED28" s="50"/>
-      <c r="EE28" s="50"/>
-      <c r="EF28" s="50"/>
-      <c r="EG28" s="50"/>
-      <c r="EH28" s="50"/>
-      <c r="EI28" s="50"/>
-      <c r="EJ28" s="50"/>
-      <c r="EK28" s="50"/>
-      <c r="EL28" s="50"/>
-      <c r="EM28" s="50"/>
-      <c r="EN28" s="50"/>
-      <c r="EO28" s="50"/>
-      <c r="EP28" s="50"/>
-      <c r="EQ28" s="50"/>
-      <c r="ER28" s="50"/>
-      <c r="ES28" s="50"/>
-      <c r="ET28" s="50"/>
-      <c r="EU28" s="50"/>
-      <c r="EV28" s="50"/>
-      <c r="EW28" s="50"/>
-      <c r="EX28" s="50"/>
-      <c r="EY28" s="50"/>
-      <c r="EZ28" s="50"/>
-      <c r="FA28" s="50"/>
-      <c r="FB28" s="50"/>
-      <c r="FC28" s="50"/>
-      <c r="FD28" s="50"/>
-      <c r="FE28" s="50"/>
-      <c r="FF28" s="50"/>
-      <c r="FG28" s="50"/>
-      <c r="FH28" s="50"/>
-      <c r="FI28" s="50"/>
-      <c r="FJ28" s="50"/>
-      <c r="FK28" s="50"/>
-      <c r="FL28" s="50"/>
-      <c r="FM28" s="50"/>
-      <c r="FN28" s="50"/>
-      <c r="FO28" s="50"/>
-      <c r="FP28" s="50"/>
-      <c r="FQ28" s="50"/>
-      <c r="FR28" s="50"/>
-      <c r="FS28" s="50"/>
-      <c r="FT28" s="50"/>
-      <c r="FU28" s="50"/>
-      <c r="FV28" s="50"/>
-      <c r="FW28" s="50"/>
-      <c r="FX28" s="50"/>
-      <c r="FY28" s="50"/>
-      <c r="FZ28" s="50"/>
-      <c r="GA28" s="50"/>
-      <c r="GB28" s="50"/>
-      <c r="GC28" s="50"/>
-      <c r="GD28" s="50"/>
-      <c r="GE28" s="50"/>
-      <c r="GF28" s="50"/>
-      <c r="GG28" s="50"/>
-      <c r="GH28" s="50"/>
-      <c r="GI28" s="50"/>
-      <c r="GJ28" s="50"/>
-      <c r="GK28" s="50"/>
-      <c r="GL28" s="50"/>
-      <c r="GM28" s="50"/>
-      <c r="GN28" s="50"/>
-      <c r="GO28" s="50"/>
-      <c r="GP28" s="50"/>
-      <c r="GQ28" s="50"/>
-      <c r="GR28" s="50"/>
-      <c r="GS28" s="50"/>
-      <c r="GT28" s="50"/>
-      <c r="GU28" s="50"/>
-      <c r="GV28" s="50"/>
-      <c r="GW28" s="50"/>
-      <c r="GX28" s="50"/>
-      <c r="GY28" s="50"/>
-      <c r="GZ28" s="50"/>
-      <c r="HA28" s="50"/>
-      <c r="HB28" s="50"/>
-      <c r="HC28" s="50"/>
-      <c r="HD28" s="50"/>
-      <c r="HE28" s="50"/>
-      <c r="HF28" s="50"/>
-      <c r="HG28" s="50"/>
-      <c r="HH28" s="50"/>
-      <c r="HI28" s="50"/>
-      <c r="HJ28" s="50"/>
-      <c r="HK28" s="50"/>
-      <c r="HL28" s="50"/>
-      <c r="HM28" s="50"/>
-      <c r="HN28" s="50"/>
-      <c r="HO28" s="50"/>
-      <c r="HP28" s="50"/>
-      <c r="HQ28" s="50"/>
-      <c r="HR28" s="50"/>
-      <c r="HS28" s="50"/>
-      <c r="HT28" s="50"/>
-      <c r="HU28" s="50"/>
-      <c r="HV28" s="50"/>
-      <c r="HW28" s="50"/>
-      <c r="HX28" s="50"/>
-      <c r="HY28" s="50"/>
-      <c r="HZ28" s="50"/>
-      <c r="IA28" s="50"/>
-      <c r="IB28" s="50"/>
-      <c r="IC28" s="50"/>
-      <c r="ID28" s="50"/>
-      <c r="IE28" s="50"/>
-      <c r="IF28" s="50"/>
-      <c r="IG28" s="50"/>
-      <c r="IH28" s="50"/>
-      <c r="II28" s="50"/>
-      <c r="IJ28" s="50"/>
-      <c r="IK28" s="50"/>
-      <c r="IL28" s="50"/>
-      <c r="IM28" s="50"/>
-      <c r="IN28" s="50"/>
-      <c r="IO28" s="50"/>
-      <c r="IP28" s="50"/>
-      <c r="IQ28" s="50"/>
-      <c r="IR28" s="50"/>
-      <c r="IS28" s="50"/>
-      <c r="IT28" s="50"/>
-      <c r="IU28" s="50"/>
-      <c r="IV28" s="50"/>
-      <c r="IW28" s="50"/>
-    </row>
-    <row r="29" ht="12.75" customHeight="1">
-      <c r="D29" s="49"/>
-      <c r="I29" s="49"/>
-    </row>
-    <row r="45" ht="12.75" customHeight="1">
-      <c r="I45" s="49"/>
-    </row>
-  </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="G6:K6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="G7:K7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:C15"/>
-    <mergeCell ref="D14:K15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:K19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:K21"/>
-  </mergeCells>
-  <dataValidations count="1" disablePrompts="0">
-    <dataValidation sqref="C2" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
-      <formula1>Sheet1!$A$1:$A$3</formula1>
-    </dataValidation>
-  </dataValidations>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="1" scale="90" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="65533" verticalDpi="65533" copies="1"/>
-  <headerFooter/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="F18" activeCellId="0" sqref="F18:K20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" customHeight="1"/>
-  <cols>
-    <col customWidth="1" min="1" max="257" style="2" width="9.1406200000000002"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="12.75">
-      <c r="A1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="8"/>
-    </row>
-    <row r="2" ht="12.75">
-      <c r="A2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" ht="12.75">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="4" ht="12.75">
-      <c r="A4" s="53" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" ht="12.75">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-    </row>
-    <row r="6" ht="12.75">
-      <c r="A6" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="22"/>
-    </row>
-    <row r="7" ht="12.75">
-      <c r="A7" s="23">
-        <v>1</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="23">
-        <v>1</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="26"/>
-    </row>
-    <row r="8" ht="12.75">
-      <c r="A8" s="27">
-        <v>2</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="27">
-        <v>2</v>
-      </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="30"/>
-    </row>
-    <row r="9" ht="12.75">
-      <c r="A9" s="27">
-        <v>3</v>
-      </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="27">
-        <v>3</v>
-      </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="30"/>
-    </row>
-    <row r="10" ht="12.75">
-      <c r="A10" s="27">
-        <v>4</v>
-      </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="27">
-        <v>4</v>
-      </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="30"/>
-    </row>
-    <row r="11" ht="12.75">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" ht="12.75">
-      <c r="A12" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="14" ht="12.75">
-      <c r="A14" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39"/>
-    </row>
-    <row r="15" ht="12.75">
-      <c r="A15" s="40"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="44"/>
-    </row>
-    <row r="16" ht="24.75" customHeight="1">
-      <c r="A16" s="23">
-        <v>1</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="26"/>
-    </row>
-    <row r="17" ht="12.75">
-      <c r="A17" s="27">
-        <v>2</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="30"/>
-    </row>
-    <row r="18" ht="12.75">
-      <c r="A18" s="27">
-        <v>3</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="30"/>
-    </row>
-    <row r="19" ht="12.75">
-      <c r="A19" s="27">
-        <v>4</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="30"/>
-    </row>
-    <row r="20" ht="12.75">
-      <c r="A20" s="27">
-        <v>5</v>
-      </c>
-      <c r="B20" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="28" t="s">
-        <v>61</v>
-      </c>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
@@ -13421,6 +13257,14 @@
       <c r="D29" s="49"/>
       <c r="H29" s="49"/>
     </row>
+    <row r="40" ht="12.75" customHeight="1">
+      <c r="H40" s="51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" ht="12.75" customHeight="1">
+      <c r="H41" s="49"/>
+    </row>
   </sheetData>
   <mergeCells count="31">
     <mergeCell ref="A1:B1"/>
@@ -13468,7 +13312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -13491,14 +13335,14 @@
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="5" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
@@ -13601,7 +13445,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -13679,7 +13523,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -13785,11 +13629,11 @@
         <v>4</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="28" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
@@ -13800,15 +13644,691 @@
       <c r="K19" s="30"/>
     </row>
     <row r="20" ht="12.75">
+      <c r="A20" s="27"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="30"/>
+    </row>
+    <row r="21" ht="12.75">
+      <c r="A21" s="27"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="30"/>
+    </row>
+    <row r="28" s="50" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A28" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="50"/>
+      <c r="V28" s="50"/>
+      <c r="W28" s="50"/>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="50"/>
+      <c r="Z28" s="50"/>
+      <c r="AA28" s="50"/>
+      <c r="AB28" s="50"/>
+      <c r="AC28" s="50"/>
+      <c r="AD28" s="50"/>
+      <c r="AE28" s="50"/>
+      <c r="AF28" s="50"/>
+      <c r="AG28" s="50"/>
+      <c r="AH28" s="50"/>
+      <c r="AI28" s="50"/>
+      <c r="AJ28" s="50"/>
+      <c r="AK28" s="50"/>
+      <c r="AL28" s="50"/>
+      <c r="AM28" s="50"/>
+      <c r="AN28" s="50"/>
+      <c r="AO28" s="50"/>
+      <c r="AP28" s="50"/>
+      <c r="AQ28" s="50"/>
+      <c r="AR28" s="50"/>
+      <c r="AS28" s="50"/>
+      <c r="AT28" s="50"/>
+      <c r="AU28" s="50"/>
+      <c r="AV28" s="50"/>
+      <c r="AW28" s="50"/>
+      <c r="AX28" s="50"/>
+      <c r="AY28" s="50"/>
+      <c r="AZ28" s="50"/>
+      <c r="BA28" s="50"/>
+      <c r="BB28" s="50"/>
+      <c r="BC28" s="50"/>
+      <c r="BD28" s="50"/>
+      <c r="BE28" s="50"/>
+      <c r="BF28" s="50"/>
+      <c r="BG28" s="50"/>
+      <c r="BH28" s="50"/>
+      <c r="BI28" s="50"/>
+      <c r="BJ28" s="50"/>
+      <c r="BK28" s="50"/>
+      <c r="BL28" s="50"/>
+      <c r="BM28" s="50"/>
+      <c r="BN28" s="50"/>
+      <c r="BO28" s="50"/>
+      <c r="BP28" s="50"/>
+      <c r="BQ28" s="50"/>
+      <c r="BR28" s="50"/>
+      <c r="BS28" s="50"/>
+      <c r="BT28" s="50"/>
+      <c r="BU28" s="50"/>
+      <c r="BV28" s="50"/>
+      <c r="BW28" s="50"/>
+      <c r="BX28" s="50"/>
+      <c r="BY28" s="50"/>
+      <c r="BZ28" s="50"/>
+      <c r="CA28" s="50"/>
+      <c r="CB28" s="50"/>
+      <c r="CC28" s="50"/>
+      <c r="CD28" s="50"/>
+      <c r="CE28" s="50"/>
+      <c r="CF28" s="50"/>
+      <c r="CG28" s="50"/>
+      <c r="CH28" s="50"/>
+      <c r="CI28" s="50"/>
+      <c r="CJ28" s="50"/>
+      <c r="CK28" s="50"/>
+      <c r="CL28" s="50"/>
+      <c r="CM28" s="50"/>
+      <c r="CN28" s="50"/>
+      <c r="CO28" s="50"/>
+      <c r="CP28" s="50"/>
+      <c r="CQ28" s="50"/>
+      <c r="CR28" s="50"/>
+      <c r="CS28" s="50"/>
+      <c r="CT28" s="50"/>
+      <c r="CU28" s="50"/>
+      <c r="CV28" s="50"/>
+      <c r="CW28" s="50"/>
+      <c r="CX28" s="50"/>
+      <c r="CY28" s="50"/>
+      <c r="CZ28" s="50"/>
+      <c r="DA28" s="50"/>
+      <c r="DB28" s="50"/>
+      <c r="DC28" s="50"/>
+      <c r="DD28" s="50"/>
+      <c r="DE28" s="50"/>
+      <c r="DF28" s="50"/>
+      <c r="DG28" s="50"/>
+      <c r="DH28" s="50"/>
+      <c r="DI28" s="50"/>
+      <c r="DJ28" s="50"/>
+      <c r="DK28" s="50"/>
+      <c r="DL28" s="50"/>
+      <c r="DM28" s="50"/>
+      <c r="DN28" s="50"/>
+      <c r="DO28" s="50"/>
+      <c r="DP28" s="50"/>
+      <c r="DQ28" s="50"/>
+      <c r="DR28" s="50"/>
+      <c r="DS28" s="50"/>
+      <c r="DT28" s="50"/>
+      <c r="DU28" s="50"/>
+      <c r="DV28" s="50"/>
+      <c r="DW28" s="50"/>
+      <c r="DX28" s="50"/>
+      <c r="DY28" s="50"/>
+      <c r="DZ28" s="50"/>
+      <c r="EA28" s="50"/>
+      <c r="EB28" s="50"/>
+      <c r="EC28" s="50"/>
+      <c r="ED28" s="50"/>
+      <c r="EE28" s="50"/>
+      <c r="EF28" s="50"/>
+      <c r="EG28" s="50"/>
+      <c r="EH28" s="50"/>
+      <c r="EI28" s="50"/>
+      <c r="EJ28" s="50"/>
+      <c r="EK28" s="50"/>
+      <c r="EL28" s="50"/>
+      <c r="EM28" s="50"/>
+      <c r="EN28" s="50"/>
+      <c r="EO28" s="50"/>
+      <c r="EP28" s="50"/>
+      <c r="EQ28" s="50"/>
+      <c r="ER28" s="50"/>
+      <c r="ES28" s="50"/>
+      <c r="ET28" s="50"/>
+      <c r="EU28" s="50"/>
+      <c r="EV28" s="50"/>
+      <c r="EW28" s="50"/>
+      <c r="EX28" s="50"/>
+      <c r="EY28" s="50"/>
+      <c r="EZ28" s="50"/>
+      <c r="FA28" s="50"/>
+      <c r="FB28" s="50"/>
+      <c r="FC28" s="50"/>
+      <c r="FD28" s="50"/>
+      <c r="FE28" s="50"/>
+      <c r="FF28" s="50"/>
+      <c r="FG28" s="50"/>
+      <c r="FH28" s="50"/>
+      <c r="FI28" s="50"/>
+      <c r="FJ28" s="50"/>
+      <c r="FK28" s="50"/>
+      <c r="FL28" s="50"/>
+      <c r="FM28" s="50"/>
+      <c r="FN28" s="50"/>
+      <c r="FO28" s="50"/>
+      <c r="FP28" s="50"/>
+      <c r="FQ28" s="50"/>
+      <c r="FR28" s="50"/>
+      <c r="FS28" s="50"/>
+      <c r="FT28" s="50"/>
+      <c r="FU28" s="50"/>
+      <c r="FV28" s="50"/>
+      <c r="FW28" s="50"/>
+      <c r="FX28" s="50"/>
+      <c r="FY28" s="50"/>
+      <c r="FZ28" s="50"/>
+      <c r="GA28" s="50"/>
+      <c r="GB28" s="50"/>
+      <c r="GC28" s="50"/>
+      <c r="GD28" s="50"/>
+      <c r="GE28" s="50"/>
+      <c r="GF28" s="50"/>
+      <c r="GG28" s="50"/>
+      <c r="GH28" s="50"/>
+      <c r="GI28" s="50"/>
+      <c r="GJ28" s="50"/>
+      <c r="GK28" s="50"/>
+      <c r="GL28" s="50"/>
+      <c r="GM28" s="50"/>
+      <c r="GN28" s="50"/>
+      <c r="GO28" s="50"/>
+      <c r="GP28" s="50"/>
+      <c r="GQ28" s="50"/>
+      <c r="GR28" s="50"/>
+      <c r="GS28" s="50"/>
+      <c r="GT28" s="50"/>
+      <c r="GU28" s="50"/>
+      <c r="GV28" s="50"/>
+      <c r="GW28" s="50"/>
+      <c r="GX28" s="50"/>
+      <c r="GY28" s="50"/>
+      <c r="GZ28" s="50"/>
+      <c r="HA28" s="50"/>
+      <c r="HB28" s="50"/>
+      <c r="HC28" s="50"/>
+      <c r="HD28" s="50"/>
+      <c r="HE28" s="50"/>
+      <c r="HF28" s="50"/>
+      <c r="HG28" s="50"/>
+      <c r="HH28" s="50"/>
+      <c r="HI28" s="50"/>
+      <c r="HJ28" s="50"/>
+      <c r="HK28" s="50"/>
+      <c r="HL28" s="50"/>
+      <c r="HM28" s="50"/>
+      <c r="HN28" s="50"/>
+      <c r="HO28" s="50"/>
+      <c r="HP28" s="50"/>
+      <c r="HQ28" s="50"/>
+      <c r="HR28" s="50"/>
+      <c r="HS28" s="50"/>
+      <c r="HT28" s="50"/>
+      <c r="HU28" s="50"/>
+      <c r="HV28" s="50"/>
+      <c r="HW28" s="50"/>
+      <c r="HX28" s="50"/>
+      <c r="HY28" s="50"/>
+      <c r="HZ28" s="50"/>
+      <c r="IA28" s="50"/>
+      <c r="IB28" s="50"/>
+      <c r="IC28" s="50"/>
+      <c r="ID28" s="50"/>
+      <c r="IE28" s="50"/>
+      <c r="IF28" s="50"/>
+      <c r="IG28" s="50"/>
+      <c r="IH28" s="50"/>
+      <c r="II28" s="50"/>
+      <c r="IJ28" s="50"/>
+      <c r="IK28" s="50"/>
+      <c r="IL28" s="50"/>
+      <c r="IM28" s="50"/>
+      <c r="IN28" s="50"/>
+      <c r="IO28" s="50"/>
+      <c r="IP28" s="50"/>
+      <c r="IQ28" s="50"/>
+      <c r="IR28" s="50"/>
+      <c r="IS28" s="50"/>
+      <c r="IT28" s="50"/>
+      <c r="IU28" s="50"/>
+      <c r="IV28" s="50"/>
+      <c r="IW28" s="50"/>
+    </row>
+    <row r="29" ht="12.75" customHeight="1">
+      <c r="D29" s="49"/>
+      <c r="I29" s="49"/>
+    </row>
+    <row r="45" ht="12.75" customHeight="1">
+      <c r="I45" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="31">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="D14:K15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:K21"/>
+  </mergeCells>
+  <dataValidations count="1" disablePrompts="0">
+    <dataValidation sqref="C2" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Sheet1!$A$1:$A$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="1" scale="90" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="65533" verticalDpi="65533" copies="1"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="F18" activeCellId="0" sqref="F18:K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" customHeight="1"/>
+  <cols>
+    <col customWidth="1" min="1" max="257" style="2" width="9.1406200000000002"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="12.75">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" ht="12.75">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" ht="12.75">
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" ht="12.75">
+      <c r="A4" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" ht="12.75">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" ht="12.75">
+      <c r="A6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="22"/>
+    </row>
+    <row r="7" ht="12.75">
+      <c r="A7" s="23">
+        <v>1</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="23">
+        <v>1</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" ht="12.75">
+      <c r="A8" s="27">
+        <v>2</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="27">
+        <v>2</v>
+      </c>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+    </row>
+    <row r="9" ht="12.75">
+      <c r="A9" s="27">
+        <v>3</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="27">
+        <v>3</v>
+      </c>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
+    </row>
+    <row r="10" ht="12.75">
+      <c r="A10" s="27">
+        <v>4</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="27">
+        <v>4</v>
+      </c>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
+    </row>
+    <row r="11" ht="12.75">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" ht="12.75">
+      <c r="A12" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="14" ht="12.75">
+      <c r="A14" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+    </row>
+    <row r="15" ht="12.75">
+      <c r="A15" s="40"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="44"/>
+    </row>
+    <row r="16" ht="24.75" customHeight="1">
+      <c r="A16" s="23">
+        <v>1</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="26"/>
+    </row>
+    <row r="17" ht="12.75">
+      <c r="A17" s="27">
+        <v>2</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
+    </row>
+    <row r="18" ht="12.75">
+      <c r="A18" s="27">
+        <v>3</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="30"/>
+    </row>
+    <row r="19" ht="12.75">
+      <c r="A19" s="27">
+        <v>4</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="30"/>
+    </row>
+    <row r="20" ht="12.75">
       <c r="A20" s="27">
         <v>5</v>
       </c>
       <c r="B20" s="47" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C20" s="48"/>
       <c r="D20" s="28" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
@@ -14100,9 +14620,6 @@
       <c r="D29" s="49"/>
       <c r="H29" s="49"/>
     </row>
-    <row r="39" ht="12.75" customHeight="1">
-      <c r="H39" s="49"/>
-    </row>
   </sheetData>
   <mergeCells count="31">
     <mergeCell ref="A1:B1"/>
@@ -14150,7 +14667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -14173,14 +14690,14 @@
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
@@ -14283,7 +14800,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="25"/>
@@ -14361,7 +14878,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -14467,11 +14984,11 @@
         <v>4</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="28" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
@@ -14482,10 +14999,16 @@
       <c r="K19" s="30"/>
     </row>
     <row r="20" ht="12.75">
-      <c r="A20" s="27"/>
-      <c r="B20" s="47"/>
+      <c r="A20" s="27">
+        <v>5</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>68</v>
+      </c>
       <c r="C20" s="48"/>
-      <c r="D20" s="28"/>
+      <c r="D20" s="28" t="s">
+        <v>69</v>
+      </c>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
@@ -14776,6 +15299,682 @@
       <c r="D29" s="49"/>
       <c r="H29" s="49"/>
     </row>
+    <row r="39" ht="12.75" customHeight="1">
+      <c r="H39" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="31">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="G6:K6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="D14:K15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:K21"/>
+  </mergeCells>
+  <dataValidations count="1" disablePrompts="0">
+    <dataValidation sqref="C2" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+      <formula1>Sheet1!$A$1:$A$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="1" scale="90" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="65533" verticalDpi="65533" copies="1"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+    <outlinePr applyStyles="0" summaryBelow="1" summaryRight="1" showOutlineSymbols="1"/>
+    <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="F18" activeCellId="0" sqref="F18:K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" customHeight="1"/>
+  <cols>
+    <col customWidth="1" min="1" max="257" style="2" width="9.1406200000000002"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="12.75">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" ht="12.75">
+      <c r="A2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" ht="12.75">
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+    </row>
+    <row r="4" ht="12.75">
+      <c r="A4" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" ht="12.75">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" ht="12.75">
+      <c r="A6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="22"/>
+    </row>
+    <row r="7" ht="12.75">
+      <c r="A7" s="23">
+        <v>1</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="23">
+        <v>1</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
+    </row>
+    <row r="8" ht="12.75">
+      <c r="A8" s="27">
+        <v>2</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="27">
+        <v>2</v>
+      </c>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+    </row>
+    <row r="9" ht="12.75">
+      <c r="A9" s="27">
+        <v>3</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="27">
+        <v>3</v>
+      </c>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="30"/>
+    </row>
+    <row r="10" ht="12.75">
+      <c r="A10" s="27">
+        <v>4</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="27">
+        <v>4</v>
+      </c>
+      <c r="G10" s="28"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="30"/>
+    </row>
+    <row r="11" ht="12.75">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" ht="12.75">
+      <c r="A12" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="14" ht="12.75">
+      <c r="A14" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="39"/>
+    </row>
+    <row r="15" ht="12.75">
+      <c r="A15" s="40"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="44"/>
+    </row>
+    <row r="16" ht="24.75" customHeight="1">
+      <c r="A16" s="23">
+        <v>1</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="26"/>
+    </row>
+    <row r="17" ht="12.75">
+      <c r="A17" s="27">
+        <v>2</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
+    </row>
+    <row r="18" ht="12.75">
+      <c r="A18" s="27">
+        <v>3</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="30"/>
+    </row>
+    <row r="19" ht="12.75">
+      <c r="A19" s="27">
+        <v>4</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="30"/>
+    </row>
+    <row r="20" ht="12.75">
+      <c r="A20" s="27"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="30"/>
+    </row>
+    <row r="21" ht="12.75">
+      <c r="A21" s="27"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="30"/>
+    </row>
+    <row r="28" s="50" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A28" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="50"/>
+      <c r="V28" s="50"/>
+      <c r="W28" s="50"/>
+      <c r="X28" s="50"/>
+      <c r="Y28" s="50"/>
+      <c r="Z28" s="50"/>
+      <c r="AA28" s="50"/>
+      <c r="AB28" s="50"/>
+      <c r="AC28" s="50"/>
+      <c r="AD28" s="50"/>
+      <c r="AE28" s="50"/>
+      <c r="AF28" s="50"/>
+      <c r="AG28" s="50"/>
+      <c r="AH28" s="50"/>
+      <c r="AI28" s="50"/>
+      <c r="AJ28" s="50"/>
+      <c r="AK28" s="50"/>
+      <c r="AL28" s="50"/>
+      <c r="AM28" s="50"/>
+      <c r="AN28" s="50"/>
+      <c r="AO28" s="50"/>
+      <c r="AP28" s="50"/>
+      <c r="AQ28" s="50"/>
+      <c r="AR28" s="50"/>
+      <c r="AS28" s="50"/>
+      <c r="AT28" s="50"/>
+      <c r="AU28" s="50"/>
+      <c r="AV28" s="50"/>
+      <c r="AW28" s="50"/>
+      <c r="AX28" s="50"/>
+      <c r="AY28" s="50"/>
+      <c r="AZ28" s="50"/>
+      <c r="BA28" s="50"/>
+      <c r="BB28" s="50"/>
+      <c r="BC28" s="50"/>
+      <c r="BD28" s="50"/>
+      <c r="BE28" s="50"/>
+      <c r="BF28" s="50"/>
+      <c r="BG28" s="50"/>
+      <c r="BH28" s="50"/>
+      <c r="BI28" s="50"/>
+      <c r="BJ28" s="50"/>
+      <c r="BK28" s="50"/>
+      <c r="BL28" s="50"/>
+      <c r="BM28" s="50"/>
+      <c r="BN28" s="50"/>
+      <c r="BO28" s="50"/>
+      <c r="BP28" s="50"/>
+      <c r="BQ28" s="50"/>
+      <c r="BR28" s="50"/>
+      <c r="BS28" s="50"/>
+      <c r="BT28" s="50"/>
+      <c r="BU28" s="50"/>
+      <c r="BV28" s="50"/>
+      <c r="BW28" s="50"/>
+      <c r="BX28" s="50"/>
+      <c r="BY28" s="50"/>
+      <c r="BZ28" s="50"/>
+      <c r="CA28" s="50"/>
+      <c r="CB28" s="50"/>
+      <c r="CC28" s="50"/>
+      <c r="CD28" s="50"/>
+      <c r="CE28" s="50"/>
+      <c r="CF28" s="50"/>
+      <c r="CG28" s="50"/>
+      <c r="CH28" s="50"/>
+      <c r="CI28" s="50"/>
+      <c r="CJ28" s="50"/>
+      <c r="CK28" s="50"/>
+      <c r="CL28" s="50"/>
+      <c r="CM28" s="50"/>
+      <c r="CN28" s="50"/>
+      <c r="CO28" s="50"/>
+      <c r="CP28" s="50"/>
+      <c r="CQ28" s="50"/>
+      <c r="CR28" s="50"/>
+      <c r="CS28" s="50"/>
+      <c r="CT28" s="50"/>
+      <c r="CU28" s="50"/>
+      <c r="CV28" s="50"/>
+      <c r="CW28" s="50"/>
+      <c r="CX28" s="50"/>
+      <c r="CY28" s="50"/>
+      <c r="CZ28" s="50"/>
+      <c r="DA28" s="50"/>
+      <c r="DB28" s="50"/>
+      <c r="DC28" s="50"/>
+      <c r="DD28" s="50"/>
+      <c r="DE28" s="50"/>
+      <c r="DF28" s="50"/>
+      <c r="DG28" s="50"/>
+      <c r="DH28" s="50"/>
+      <c r="DI28" s="50"/>
+      <c r="DJ28" s="50"/>
+      <c r="DK28" s="50"/>
+      <c r="DL28" s="50"/>
+      <c r="DM28" s="50"/>
+      <c r="DN28" s="50"/>
+      <c r="DO28" s="50"/>
+      <c r="DP28" s="50"/>
+      <c r="DQ28" s="50"/>
+      <c r="DR28" s="50"/>
+      <c r="DS28" s="50"/>
+      <c r="DT28" s="50"/>
+      <c r="DU28" s="50"/>
+      <c r="DV28" s="50"/>
+      <c r="DW28" s="50"/>
+      <c r="DX28" s="50"/>
+      <c r="DY28" s="50"/>
+      <c r="DZ28" s="50"/>
+      <c r="EA28" s="50"/>
+      <c r="EB28" s="50"/>
+      <c r="EC28" s="50"/>
+      <c r="ED28" s="50"/>
+      <c r="EE28" s="50"/>
+      <c r="EF28" s="50"/>
+      <c r="EG28" s="50"/>
+      <c r="EH28" s="50"/>
+      <c r="EI28" s="50"/>
+      <c r="EJ28" s="50"/>
+      <c r="EK28" s="50"/>
+      <c r="EL28" s="50"/>
+      <c r="EM28" s="50"/>
+      <c r="EN28" s="50"/>
+      <c r="EO28" s="50"/>
+      <c r="EP28" s="50"/>
+      <c r="EQ28" s="50"/>
+      <c r="ER28" s="50"/>
+      <c r="ES28" s="50"/>
+      <c r="ET28" s="50"/>
+      <c r="EU28" s="50"/>
+      <c r="EV28" s="50"/>
+      <c r="EW28" s="50"/>
+      <c r="EX28" s="50"/>
+      <c r="EY28" s="50"/>
+      <c r="EZ28" s="50"/>
+      <c r="FA28" s="50"/>
+      <c r="FB28" s="50"/>
+      <c r="FC28" s="50"/>
+      <c r="FD28" s="50"/>
+      <c r="FE28" s="50"/>
+      <c r="FF28" s="50"/>
+      <c r="FG28" s="50"/>
+      <c r="FH28" s="50"/>
+      <c r="FI28" s="50"/>
+      <c r="FJ28" s="50"/>
+      <c r="FK28" s="50"/>
+      <c r="FL28" s="50"/>
+      <c r="FM28" s="50"/>
+      <c r="FN28" s="50"/>
+      <c r="FO28" s="50"/>
+      <c r="FP28" s="50"/>
+      <c r="FQ28" s="50"/>
+      <c r="FR28" s="50"/>
+      <c r="FS28" s="50"/>
+      <c r="FT28" s="50"/>
+      <c r="FU28" s="50"/>
+      <c r="FV28" s="50"/>
+      <c r="FW28" s="50"/>
+      <c r="FX28" s="50"/>
+      <c r="FY28" s="50"/>
+      <c r="FZ28" s="50"/>
+      <c r="GA28" s="50"/>
+      <c r="GB28" s="50"/>
+      <c r="GC28" s="50"/>
+      <c r="GD28" s="50"/>
+      <c r="GE28" s="50"/>
+      <c r="GF28" s="50"/>
+      <c r="GG28" s="50"/>
+      <c r="GH28" s="50"/>
+      <c r="GI28" s="50"/>
+      <c r="GJ28" s="50"/>
+      <c r="GK28" s="50"/>
+      <c r="GL28" s="50"/>
+      <c r="GM28" s="50"/>
+      <c r="GN28" s="50"/>
+      <c r="GO28" s="50"/>
+      <c r="GP28" s="50"/>
+      <c r="GQ28" s="50"/>
+      <c r="GR28" s="50"/>
+      <c r="GS28" s="50"/>
+      <c r="GT28" s="50"/>
+      <c r="GU28" s="50"/>
+      <c r="GV28" s="50"/>
+      <c r="GW28" s="50"/>
+      <c r="GX28" s="50"/>
+      <c r="GY28" s="50"/>
+      <c r="GZ28" s="50"/>
+      <c r="HA28" s="50"/>
+      <c r="HB28" s="50"/>
+      <c r="HC28" s="50"/>
+      <c r="HD28" s="50"/>
+      <c r="HE28" s="50"/>
+      <c r="HF28" s="50"/>
+      <c r="HG28" s="50"/>
+      <c r="HH28" s="50"/>
+      <c r="HI28" s="50"/>
+      <c r="HJ28" s="50"/>
+      <c r="HK28" s="50"/>
+      <c r="HL28" s="50"/>
+      <c r="HM28" s="50"/>
+      <c r="HN28" s="50"/>
+      <c r="HO28" s="50"/>
+      <c r="HP28" s="50"/>
+      <c r="HQ28" s="50"/>
+      <c r="HR28" s="50"/>
+      <c r="HS28" s="50"/>
+      <c r="HT28" s="50"/>
+      <c r="HU28" s="50"/>
+      <c r="HV28" s="50"/>
+      <c r="HW28" s="50"/>
+      <c r="HX28" s="50"/>
+      <c r="HY28" s="50"/>
+      <c r="HZ28" s="50"/>
+      <c r="IA28" s="50"/>
+      <c r="IB28" s="50"/>
+      <c r="IC28" s="50"/>
+      <c r="ID28" s="50"/>
+      <c r="IE28" s="50"/>
+      <c r="IF28" s="50"/>
+      <c r="IG28" s="50"/>
+      <c r="IH28" s="50"/>
+      <c r="II28" s="50"/>
+      <c r="IJ28" s="50"/>
+      <c r="IK28" s="50"/>
+      <c r="IL28" s="50"/>
+      <c r="IM28" s="50"/>
+      <c r="IN28" s="50"/>
+      <c r="IO28" s="50"/>
+      <c r="IP28" s="50"/>
+      <c r="IQ28" s="50"/>
+      <c r="IR28" s="50"/>
+      <c r="IS28" s="50"/>
+      <c r="IT28" s="50"/>
+      <c r="IU28" s="50"/>
+      <c r="IV28" s="50"/>
+      <c r="IW28" s="50"/>
+    </row>
+    <row r="29" ht="12.75" customHeight="1">
+      <c r="D29" s="49"/>
+      <c r="H29" s="49"/>
+    </row>
   </sheetData>
   <mergeCells count="31">
     <mergeCell ref="A1:B1"/>

</xml_diff>